<commit_message>
Sir Tomato sprite update
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>water pUddle</t>
+  </si>
+  <si>
+    <t>Lava puddle</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,6 +652,12 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
       <c r="E14" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
first update for sirtomato
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lekes\Documents\GitHub\pizzatales\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\pizzat\pizzatales\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12108" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12105" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -165,12 +165,18 @@
   </si>
   <si>
     <t>l</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -491,25 +497,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -523,7 +529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -537,7 +543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -551,7 +557,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -565,7 +571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>16</v>
       </c>
@@ -573,7 +579,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -587,7 +593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -595,7 +601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -609,7 +615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -623,7 +629,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -637,7 +643,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -651,7 +657,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -665,12 +671,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>30</v>
       </c>
       <c r="F15" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
L24 and lava damage
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -179,10 +179,16 @@
     <t>cave Exit</t>
   </si>
   <si>
-    <t>Finish block</t>
-  </si>
-  <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>Arena centering target</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>water flOw</t>
   </si>
 </sst>
 </file>
@@ -509,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,10 +715,18 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
-        <v>52</v>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding levelexit, player initial position, basic level loading, pause
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lekes\Documents\GitHub\pizzatales\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\pizzat\pizzatales\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12108" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12105" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -189,12 +189,27 @@
   </si>
   <si>
     <t>water flOw</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Exit to next map</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,25 +530,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -547,7 +562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -561,7 +576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -575,7 +590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -589,7 +604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>16</v>
       </c>
@@ -597,7 +612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -611,7 +626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -619,7 +634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -633,7 +648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -647,7 +662,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -661,7 +676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -675,7 +690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -689,7 +704,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -703,17 +718,26 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
       <c r="B17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -721,12 +745,20 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
       <c r="B19" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding hidden areas management
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -204,6 +204,18 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>hidden area center</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>hidden area trigger</t>
   </si>
 </sst>
 </file>
@@ -530,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,6 +773,22 @@
         <v>59</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
implementing x scrolling + decoy correction
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lekes\Documents\GitHub\pizzatales\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\pizzat\pizzatales\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12108" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12105" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -246,12 +246,24 @@
   </si>
   <si>
     <t>decoy</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -572,25 +584,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -604,12 +616,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -618,12 +630,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -632,12 +644,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -646,7 +658,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
       <c r="E7" t="s">
         <v>16</v>
       </c>
@@ -654,12 +672,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
@@ -668,20 +686,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
@@ -690,12 +708,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
         <v>23</v>
@@ -704,12 +722,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -718,12 +736,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
         <v>26</v>
@@ -732,12 +747,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
@@ -746,12 +761,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
         <v>30</v>
@@ -760,20 +775,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
         <v>56</v>
@@ -782,84 +794,97 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>58</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>60</v>
       </c>
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
+      <c r="B29" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
background management update, scrolling stopped when reaching a limit of map, barrels added with destroyabletiles
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>barrel</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,6 +814,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
       <c r="B20" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
L41, and loads of new assets
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\pizzat\pizzatales\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lekes\Documents\GitHub\pizzatales\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12105" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12108" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -261,12 +261,72 @@
   </si>
   <si>
     <t>barrel</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>enemies</t>
+  </si>
+  <si>
+    <t>blocks</t>
+  </si>
+  <si>
+    <t>cratE</t>
+  </si>
+  <si>
+    <t>canDelabrum</t>
+  </si>
+  <si>
+    <t>cHest</t>
+  </si>
+  <si>
+    <t>Carpet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -587,95 +647,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
       </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
       </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
       </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
       </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
       <c r="E7" t="s">
         <v>16</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -688,16 +798,22 @@
       <c r="F8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -710,8 +826,11 @@
       <c r="F10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -724,8 +843,11 @@
       <c r="F11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -738,8 +860,11 @@
       <c r="F12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>74</v>
       </c>
@@ -749,8 +874,11 @@
       <c r="F13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -763,8 +891,11 @@
       <c r="F14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -777,16 +908,22 @@
       <c r="F15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>63</v>
       </c>
       <c r="B16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>75</v>
       </c>
@@ -796,105 +933,144 @@
       <c r="F17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>54</v>
       </c>
       <c r="B18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>78</v>
       </c>
       <c r="B20" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>41</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>58</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>73</v>
       </c>
       <c r="B28" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>60</v>
       </c>
       <c r="B29" t="s">
         <v>77</v>
       </c>
+      <c r="I29" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
area 5 item and tile sprites
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="105">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -324,6 +324,21 @@
   </si>
   <si>
     <t>black</t>
+  </si>
+  <si>
+    <t>pinetree</t>
+  </si>
+  <si>
+    <t>snowrock</t>
+  </si>
+  <si>
+    <t>snow</t>
+  </si>
+  <si>
+    <t>mudwall</t>
+  </si>
+  <si>
+    <t>ice</t>
   </si>
 </sst>
 </file>
@@ -367,9 +382,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,7 +669,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +834,13 @@
       <c r="B9" t="s">
         <v>51</v>
       </c>
-      <c r="I9" t="s">
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -829,6 +851,12 @@
       <c r="B10" t="s">
         <v>67</v>
       </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>88</v>
+      </c>
       <c r="E10" t="s">
         <v>22</v>
       </c>
@@ -846,6 +874,12 @@
       <c r="B11" t="s">
         <v>32</v>
       </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
       <c r="E11" t="s">
         <v>23</v>
       </c>
@@ -863,13 +897,19 @@
       <c r="B12" t="s">
         <v>47</v>
       </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
       <c r="E12" t="s">
         <v>24</v>
       </c>
       <c r="F12" t="s">
         <v>25</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -877,13 +917,19 @@
       <c r="B13" t="s">
         <v>74</v>
       </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
       <c r="E13" t="s">
         <v>26</v>
       </c>
       <c r="F13" t="s">
         <v>27</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -942,7 +988,7 @@
       <c r="F17" t="s">
         <v>57</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -975,7 +1021,7 @@
       <c r="B20" t="s">
         <v>76</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1030,7 +1076,7 @@
       <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="1" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
boosts as items and effects
</commit_message>
<xml_diff>
--- a/src/data/blocktypes.xlsx
+++ b/src/data/blocktypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="116">
   <si>
     <t>PizzaTales blocks</t>
   </si>
@@ -360,6 +360,18 @@
   </si>
   <si>
     <t>mountain floor</t>
+  </si>
+  <si>
+    <t>Cheese boost</t>
+  </si>
+  <si>
+    <t>Bacon boost</t>
+  </si>
+  <si>
+    <t>Garlic boost</t>
+  </si>
+  <si>
+    <t>Basil boost</t>
   </si>
 </sst>
 </file>
@@ -688,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,6 +1139,12 @@
       <c r="B24" t="s">
         <v>7</v>
       </c>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
       <c r="H24" t="s">
         <v>57</v>
       </c>
@@ -1138,6 +1156,12 @@
       <c r="B25" t="s">
         <v>72</v>
       </c>
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
       <c r="I25" s="1" t="s">
         <v>89</v>
       </c>
@@ -1149,6 +1173,12 @@
       <c r="B26" t="s">
         <v>4</v>
       </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
       <c r="H26" t="s">
         <v>21</v>
       </c>
@@ -1159,6 +1189,12 @@
       </c>
       <c r="B27" t="s">
         <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>90</v>

</xml_diff>